<commit_message>
feat: add some modiffy
</commit_message>
<xml_diff>
--- a/docs/学习任务书.xlsx
+++ b/docs/学习任务书.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28125" windowHeight="12540"/>
+    <workbookView windowWidth="28125" windowHeight="14340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="BlinkMacSystemFont"/>
+        <charset val="134"/>
+      </rPr>
       <t>1.配置nodejs环境；</t>
     </r>
     <r>
@@ -157,6 +163,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="BlinkMacSystemFont"/>
+        <charset val="134"/>
+      </rPr>
       <t>1.指定时间内用户再次登录不需要输入信息</t>
     </r>
     <r>
@@ -194,6 +206,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="BlinkMacSystemFont"/>
+        <charset val="134"/>
+      </rPr>
       <t>1.退出登录跳转到登录页</t>
     </r>
     <r>
@@ -231,6 +249,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="BlinkMacSystemFont"/>
+        <charset val="134"/>
+      </rPr>
       <t>1.进入首页进入发布文章可保存文本文章信息</t>
     </r>
     <r>
@@ -258,6 +282,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="BlinkMacSystemFont"/>
+        <charset val="134"/>
+      </rPr>
       <t>1.安装时间转换模块 npm install moment -g</t>
     </r>
     <r>
@@ -311,6 +341,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="BlinkMacSystemFont"/>
+        <charset val="134"/>
+      </rPr>
       <t>1.首页views/index.ejs新增分页查询参数传入</t>
     </r>
     <r>
@@ -364,6 +400,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="BlinkMacSystemFont"/>
+        <charset val="134"/>
+      </rPr>
       <t>1.点击修改进入修改页；</t>
     </r>
     <r>
@@ -429,7 +471,7 @@
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -451,13 +493,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -472,16 +507,94 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -494,23 +607,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -523,83 +635,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -616,13 +651,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -634,169 +831,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -841,21 +876,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -870,13 +890,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -899,16 +923,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="double">
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="double">
+      <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
+      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -922,153 +946,164 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1444,7 +1479,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
@@ -1500,7 +1535,7 @@
       <c r="G2" s="2"/>
       <c r="H2" s="4"/>
     </row>
-    <row r="3" ht="120" spans="1:8">
+    <row r="3" ht="127.5" spans="1:8">
       <c r="A3" s="2"/>
       <c r="B3" s="3">
         <v>2</v>
@@ -1522,7 +1557,7 @@
       </c>
       <c r="H3" s="4"/>
     </row>
-    <row r="4" ht="72" spans="1:8">
+    <row r="4" ht="76.5" spans="1:8">
       <c r="A4" s="2"/>
       <c r="B4" s="3">
         <v>3</v>
@@ -1544,7 +1579,7 @@
       </c>
       <c r="H4" s="4"/>
     </row>
-    <row r="5" ht="24" spans="1:8">
+    <row r="5" ht="25.5" spans="1:8">
       <c r="A5" s="2"/>
       <c r="B5" s="3">
         <v>4</v>
@@ -1564,7 +1599,7 @@
       </c>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" ht="48" spans="1:8">
+    <row r="6" ht="51" spans="1:8">
       <c r="A6" s="2"/>
       <c r="B6" s="3">
         <v>5</v>
@@ -1586,7 +1621,7 @@
       </c>
       <c r="H6" s="4"/>
     </row>
-    <row r="7" ht="48" spans="1:8">
+    <row r="7" ht="51" spans="1:8">
       <c r="A7" s="2"/>
       <c r="B7" s="3">
         <v>6</v>
@@ -1608,7 +1643,7 @@
       </c>
       <c r="H7" s="4"/>
     </row>
-    <row r="8" ht="60" spans="1:8">
+    <row r="8" ht="63.75" spans="1:8">
       <c r="A8" s="2"/>
       <c r="B8" s="3">
         <v>7</v>
@@ -1630,7 +1665,7 @@
       </c>
       <c r="H8" s="4"/>
     </row>
-    <row r="9" ht="36" spans="1:8">
+    <row r="9" ht="38.25" spans="1:8">
       <c r="A9" s="2"/>
       <c r="B9" s="3">
         <v>8</v>
@@ -1652,7 +1687,7 @@
       </c>
       <c r="H9" s="4"/>
     </row>
-    <row r="10" ht="24" spans="1:8">
+    <row r="10" ht="25.5" spans="1:8">
       <c r="A10" s="2"/>
       <c r="B10" s="3">
         <v>9</v>
@@ -1674,7 +1709,7 @@
       </c>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" ht="36" spans="1:8">
+    <row r="11" ht="38.25" spans="1:8">
       <c r="A11" s="2"/>
       <c r="B11" s="3">
         <v>10</v>
@@ -1694,7 +1729,7 @@
       </c>
       <c r="H11" s="4"/>
     </row>
-    <row r="12" ht="48" spans="1:8">
+    <row r="12" ht="51" spans="1:8">
       <c r="A12" s="2"/>
       <c r="B12" s="3">
         <v>11</v>
@@ -1716,7 +1751,7 @@
       </c>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" ht="36" spans="1:8">
+    <row r="13" ht="38.25" spans="1:8">
       <c r="A13" s="2"/>
       <c r="B13" s="3">
         <v>12</v>
@@ -1738,7 +1773,7 @@
       </c>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" ht="48" spans="1:8">
+    <row r="14" ht="51" spans="1:8">
       <c r="A14" s="2"/>
       <c r="B14" s="3">
         <v>13</v>

</xml_diff>